<commit_message>
Excel File Name Changed
</commit_message>
<xml_diff>
--- a/ADARSH_KOTAGIRI/RE_FRAME_WORK_FRUIT_PROJECT/Data/Config.xlsx
+++ b/ADARSH_KOTAGIRI/RE_FRAME_WORK_FRUIT_PROJECT/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\USE_Cases\RE_FRAME_WORK_FRUIT_PROJECT\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\RPA-Developer-in-30-Days\ADARSH_KOTAGIRI\RE_FRAME_WORK_FRUIT_PROJECT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -164,13 +164,13 @@
     <t>Excel_File</t>
   </si>
   <si>
-    <t>Fruits.xlsx</t>
-  </si>
-  <si>
     <t>Taste_Url</t>
   </si>
   <si>
     <t>https://www.taste.com.au</t>
+  </si>
+  <si>
+    <t>InputFruits.xlsx</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -641,15 +641,15 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>